<commit_message>
Fixed parser error for reaching endfile before using the default lenght. Added compatibility for default cases in the different lenght code.
</commit_message>
<xml_diff>
--- a/scripts_python/references/data_pair.xlsx
+++ b/scripts_python/references/data_pair.xlsx
@@ -161,15 +161,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -287,7 +278,7 @@
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3:J11"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,13 +423,13 @@
         <v>0.402246234516001</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>3.72041501963349</v>
-      </c>
-      <c r="I4" s="0" t="n">
+        <v>8.42086361836311</v>
+      </c>
+      <c r="I4" s="2" t="n">
         <v>0.501745677347789</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>21.9024301921799</v>
+        <v>30.3226130668644</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0.377268211971313</v>
@@ -461,8 +452,8 @@
       <c r="Q4" s="2" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="R4" s="2" t="n">
-        <v>-0.0732498981429615</v>
+      <c r="R4" s="0" t="n">
+        <v>6.4454799520623</v>
       </c>
       <c r="S4" s="2" t="n">
         <v>0.377268211971313</v>
@@ -506,13 +497,13 @@
         <v>0.45058944405295</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>-21.8630463943047</v>
-      </c>
-      <c r="I5" s="0" t="n">
+        <v>-17.3816690803508</v>
+      </c>
+      <c r="I5" s="2" t="n">
         <v>0.551214899264904</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>8.77959884853931</v>
+        <v>15.7495765908952</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0.402246234516001</v>
@@ -535,8 +526,8 @@
       <c r="Q5" s="2" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="R5" s="2" t="n">
-        <v>-0.745635095987069</v>
+      <c r="R5" s="0" t="n">
+        <v>3.03631159640739</v>
       </c>
       <c r="S5" s="2" t="n">
         <v>0.402246234516001</v>
@@ -580,13 +571,13 @@
         <v>0.501745677347789</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>-36.9355725932731</v>
-      </c>
-      <c r="I6" s="0" t="n">
+        <v>-28.8301741809225</v>
+      </c>
+      <c r="I6" s="2" t="n">
         <v>0.599313443125452</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>-10.0450066400899</v>
+        <v>1.18341586593766</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0.45058944405295</v>
@@ -609,8 +600,8 @@
       <c r="Q6" s="2" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="R6" s="2" t="n">
-        <v>-4.22215348946051</v>
+      <c r="R6" s="0" t="n">
+        <v>-2.52128815370404</v>
       </c>
       <c r="S6" s="2" t="n">
         <v>0.45058944405295</v>
@@ -654,13 +645,13 @@
         <v>0.551214899264904</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>-43.785860379272</v>
-      </c>
-      <c r="I7" s="0" t="n">
+        <v>-38.1864536660425</v>
+      </c>
+      <c r="I7" s="2" t="n">
         <v>0.650493343520364</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>-19.5865269493227</v>
+        <v>-9.65875567903714</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0.501745677347789</v>
@@ -683,8 +674,8 @@
       <c r="Q7" s="2" t="n">
         <v>0.551214899264904</v>
       </c>
-      <c r="R7" s="2" t="n">
-        <v>-11.9524247545846</v>
+      <c r="R7" s="0" t="n">
+        <v>-13.38605712023</v>
       </c>
       <c r="S7" s="2" t="n">
         <v>0.501745677347789</v>
@@ -728,13 +719,13 @@
         <v>0.599313443125452</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>-34.3486454641001</v>
-      </c>
-      <c r="I8" s="0" t="n">
+        <v>-36.3227021182072</v>
+      </c>
+      <c r="I8" s="2" t="n">
         <v>0.675648581248717</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>-18.2965008651382</v>
+        <v>-13.220752169069</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>0.551214899264904</v>
@@ -757,8 +748,8 @@
       <c r="Q8" s="2" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="R8" s="2" t="n">
-        <v>-10.3567475132982</v>
+      <c r="R8" s="0" t="n">
+        <v>-18.4480822544681</v>
       </c>
       <c r="S8" s="2" t="n">
         <v>0.551214899264904</v>
@@ -795,20 +786,20 @@
       <c r="E9" s="2" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>46.6272780874236</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0.650493343520364</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>5.07598266712586</v>
-      </c>
-      <c r="I9" s="0" t="n">
+        <v>-9.55303290539078</v>
+      </c>
+      <c r="I9" s="2" t="n">
         <v>0.700545785025913</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>-11.5606569352303</v>
+        <v>-13.5604847402453</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>0.599313443125452</v>
@@ -831,8 +822,8 @@
       <c r="Q9" s="2" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="R9" s="2" t="n">
-        <v>7.46112312882138</v>
+      <c r="R9" s="0" t="n">
+        <v>-20.201057990232</v>
       </c>
       <c r="S9" s="2" t="n">
         <v>0.599313443125452</v>
@@ -869,20 +860,20 @@
       <c r="E10" s="2" t="n">
         <v>0.700545785025913</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>4.50871399467582</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0.700545785025913</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>46.0697845659259</v>
-      </c>
-      <c r="I10" s="0" t="n">
+        <v>24.0593238332205</v>
+      </c>
+      <c r="I10" s="2" t="n">
         <v>0.749644859282492</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>24.04555113921</v>
+        <v>-0.058513534306087</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>0.650493343520364</v>
@@ -905,8 +896,8 @@
       <c r="Q10" s="2" t="n">
         <v>0.700545785025913</v>
       </c>
-      <c r="R10" s="2" t="n">
-        <v>45.1225877589467</v>
+      <c r="R10" s="0" t="n">
+        <v>-7.21322551882105</v>
       </c>
       <c r="S10" s="2" t="n">
         <v>0.650493343520364</v>
@@ -946,11 +937,11 @@
       <c r="F11" s="2" t="n">
         <v>-24.9759591849755</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="2" t="n">
         <v>0.801917215853616</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>77.7379015906283</v>
+        <v>21.3194301272472</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>0.700545785025913</v>

</xml_diff>

<commit_message>
edited so works without pairwise.
</commit_message>
<xml_diff>
--- a/scripts_python/references/data_pair.xlsx
+++ b/scripts_python/references/data_pair.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t xml:space="preserve">Cell</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">bccAB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaTiO3b</t>
   </si>
   <si>
     <t xml:space="preserve">Gamma</t>
@@ -139,16 +142,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,13 +274,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1048576"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -325,734 +324,743 @@
       <c r="W2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="Y2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>0.377268211971313</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <v>-39.6364566246886</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>161.019986123244</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="1" t="n">
         <v>231.824741057895</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>8.42086361836311</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>30.3226130668644</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.377268211971313</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="1" t="n">
         <v>-6.08842452781781</v>
       </c>
-      <c r="M4" s="2" t="n">
+      <c r="M4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="N4" s="2" t="n">
+      <c r="N4" s="1" t="n">
         <v>160.822514656584</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="O4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="P4" s="2" t="n">
+      <c r="P4" s="1" t="n">
         <v>64.7884351467825</v>
       </c>
-      <c r="Q4" s="2" t="n">
+      <c r="Q4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>6.4454799520623</v>
       </c>
-      <c r="S4" s="2" t="n">
+      <c r="S4" s="1" t="n">
         <v>0.377268211971313</v>
       </c>
-      <c r="T4" s="2" t="n">
+      <c r="T4" s="1" t="n">
         <v>-8.38592433619596</v>
       </c>
-      <c r="U4" s="2" t="n">
+      <c r="U4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="V4" s="2" t="n">
+      <c r="V4" s="1" t="n">
         <v>60.1183511018581</v>
       </c>
-      <c r="W4" s="2" t="n">
+      <c r="W4" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="X4" s="2" t="n">
+      <c r="X4" s="1" t="n">
         <v>-11.797334123625</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="1" t="n">
         <v>-42.724633699105</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.474076185319933</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>122.547474237137</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="1" t="n">
         <v>214.845341483955</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>-17.3816690803508</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="I5" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>15.7495765908952</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="L5" s="1" t="n">
         <v>2.02625003989006</v>
       </c>
-      <c r="M5" s="2" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="N5" s="2" t="n">
+      <c r="N5" s="1" t="n">
         <v>134.930124880778</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="O5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="P5" s="2" t="n">
+      <c r="P5" s="1" t="n">
         <v>67.5607014174319</v>
       </c>
-      <c r="Q5" s="2" t="n">
+      <c r="Q5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="1" t="n">
         <v>3.03631159640739</v>
       </c>
-      <c r="S5" s="2" t="n">
+      <c r="S5" s="1" t="n">
         <v>0.402246234516001</v>
       </c>
-      <c r="T5" s="2" t="n">
+      <c r="T5" s="1" t="n">
         <v>-15.6737789899068</v>
       </c>
-      <c r="U5" s="2" t="n">
+      <c r="U5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="V5" s="2" t="n">
+      <c r="V5" s="1" t="n">
         <v>73.3005831763657</v>
       </c>
-      <c r="W5" s="2" t="n">
+      <c r="W5" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="X5" s="2" t="n">
+      <c r="X5" s="1" t="n">
         <v>-4.72086426668943</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="1" t="n">
         <v>-42.6197259321041</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="D6" s="2" t="n">
+      <c r="C6" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>79.9745614989868</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1" t="n">
         <v>184.294985284119</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>-28.8301741809225</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <v>1.18341586593766</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="L6" s="1" t="n">
         <v>23.5603214319053</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="M6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="N6" s="1" t="n">
         <v>106.353887540727</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="O6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="P6" s="2" t="n">
+      <c r="P6" s="1" t="n">
         <v>74.2029552185333</v>
       </c>
-      <c r="Q6" s="2" t="n">
+      <c r="Q6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>-2.52128815370404</v>
       </c>
-      <c r="S6" s="2" t="n">
+      <c r="S6" s="1" t="n">
         <v>0.45058944405295</v>
       </c>
-      <c r="T6" s="2" t="n">
+      <c r="T6" s="1" t="n">
         <v>-18.2797139747718</v>
       </c>
-      <c r="U6" s="2" t="n">
+      <c r="U6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="V6" s="2" t="n">
+      <c r="V6" s="1" t="n">
         <v>104.544222584496</v>
       </c>
-      <c r="W6" s="2" t="n">
+      <c r="W6" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="X6" s="2" t="n">
+      <c r="X6" s="1" t="n">
         <v>6.49720974385676</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <v>-34.2968465340919</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.625057060568896</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>46.626465330269</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="E7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>141.517556110857</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="G7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>-38.1864536660425</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <v>-9.65875567903714</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="L7" s="1" t="n">
         <v>49.5582006937248</v>
       </c>
-      <c r="M7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="N7" s="2" t="n">
+      <c r="M7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="N7" s="1" t="n">
         <v>79.4033593012416</v>
       </c>
-      <c r="O7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="P7" s="2" t="n">
+      <c r="O7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="P7" s="1" t="n">
         <v>76.5604225622389</v>
       </c>
-      <c r="Q7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="R7" s="0" t="n">
+      <c r="Q7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="R7" s="1" t="n">
         <v>-13.38605712023</v>
       </c>
-      <c r="S7" s="2" t="n">
+      <c r="S7" s="1" t="n">
         <v>0.501745677347789</v>
       </c>
-      <c r="T7" s="2" t="n">
+      <c r="T7" s="1" t="n">
         <v>-3.18505608213079</v>
       </c>
-      <c r="U7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="V7" s="2" t="n">
+      <c r="U7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="V7" s="1" t="n">
         <v>147.555953234711</v>
       </c>
-      <c r="W7" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="X7" s="2" t="n">
+      <c r="W7" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="X7" s="1" t="n">
         <v>21.974727796534</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="B8" s="2" t="n">
+      <c r="A8" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>-13.4096106891467</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="D8" s="2" t="n">
+      <c r="C8" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>27.2613795225119</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="1" t="n">
         <v>93.9007456754996</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>-36.3227021182072</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="1" t="n">
         <v>0.675648581248717</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <v>-13.220752169069</v>
       </c>
-      <c r="K8" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="L8" s="2" t="n">
+      <c r="K8" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="L8" s="1" t="n">
         <v>76.835692739158</v>
       </c>
-      <c r="M8" s="2" t="n">
+      <c r="M8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="N8" s="2" t="n">
+      <c r="N8" s="1" t="n">
         <v>57.3544905760993</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="O8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="P8" s="2" t="n">
+      <c r="P8" s="1" t="n">
         <v>77.1196697962292</v>
       </c>
-      <c r="Q8" s="2" t="n">
+      <c r="Q8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="R8" s="1" t="n">
         <v>-18.4480822544681</v>
       </c>
-      <c r="S8" s="2" t="n">
-        <v>0.551214899264904</v>
-      </c>
-      <c r="T8" s="2" t="n">
+      <c r="S8" s="1" t="n">
+        <v>0.551214899264904</v>
+      </c>
+      <c r="T8" s="1" t="n">
         <v>33.3650612768439</v>
       </c>
-      <c r="U8" s="2" t="n">
+      <c r="U8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="V8" s="2" t="n">
+      <c r="V8" s="1" t="n">
         <v>204.23848534782</v>
       </c>
-      <c r="W8" s="2" t="n">
+      <c r="W8" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="X8" s="2" t="n">
+      <c r="X8" s="1" t="n">
         <v>42.5763193550883</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="1" t="n">
         <v>16.8011533353846</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.729293307111268</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="1" t="n">
         <v>24.8023460804507</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="1" t="n">
         <v>46.6272780874236</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>-9.55303290539078</v>
       </c>
-      <c r="I9" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="J9" s="0" t="n">
+      <c r="I9" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="J9" s="1" t="n">
         <v>-13.5604847402453</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="K9" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="L9" s="1" t="n">
         <v>98.2427899825875</v>
       </c>
-      <c r="M9" s="2" t="n">
+      <c r="M9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="N9" s="1" t="n">
         <v>38.7868419577012</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="O9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="P9" s="2" t="n">
+      <c r="P9" s="1" t="n">
         <v>73.8307167431654</v>
       </c>
-      <c r="Q9" s="2" t="n">
+      <c r="Q9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="1" t="n">
         <v>-20.201057990232</v>
       </c>
-      <c r="S9" s="2" t="n">
+      <c r="S9" s="1" t="n">
         <v>0.599313443125452</v>
       </c>
-      <c r="T9" s="2" t="n">
+      <c r="T9" s="1" t="n">
         <v>94.015203728521</v>
       </c>
-      <c r="U9" s="2" t="n">
+      <c r="U9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="V9" s="2" t="n">
+      <c r="V9" s="1" t="n">
         <v>267.378279412741</v>
       </c>
-      <c r="W9" s="2" t="n">
+      <c r="W9" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="X9" s="2" t="n">
+      <c r="X9" s="1" t="n">
         <v>77.0063867543152</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="1" t="n">
         <v>61.384805305493</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.761787315617629</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="1" t="n">
         <v>23.0834977555186</v>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="F10" s="2" t="n">
+      <c r="E10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>4.50871399467582</v>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="G10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>24.0593238332205</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="1" t="n">
         <v>0.749644859282492</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <v>-0.058513534306087</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="L10" s="2" t="n">
+      <c r="L10" s="1" t="n">
         <v>108.563000072246</v>
       </c>
-      <c r="M10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="N10" s="2" t="n">
+      <c r="M10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="N10" s="1" t="n">
         <v>28.8643330596648</v>
       </c>
-      <c r="O10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="P10" s="2" t="n">
+      <c r="O10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="P10" s="1" t="n">
         <v>66.9322868110933</v>
       </c>
-      <c r="Q10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="R10" s="0" t="n">
+      <c r="Q10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="R10" s="1" t="n">
         <v>-7.21322551882105</v>
       </c>
-      <c r="S10" s="2" t="n">
+      <c r="S10" s="1" t="n">
         <v>0.650493343520364</v>
       </c>
-      <c r="T10" s="2" t="n">
+      <c r="T10" s="1" t="n">
         <v>182.481907602592</v>
       </c>
-      <c r="U10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="V10" s="2" t="n">
+      <c r="U10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="V10" s="1" t="n">
         <v>323.603844166286</v>
       </c>
-      <c r="W10" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="X10" s="2" t="n">
+      <c r="W10" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="X10" s="1" t="n">
         <v>134.89388390567</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="B11" s="2" t="n">
+      <c r="A11" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>113.401842052341</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="1" t="n">
         <v>0.801917215853616</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="1" t="n">
         <v>24.7233358945436</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="1" t="n">
         <v>0.749644859282492</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="1" t="n">
         <v>-24.9759591849755</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="1" t="n">
         <v>0.801917215853616</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="1" t="n">
         <v>21.3194301272472</v>
       </c>
-      <c r="K11" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="L11" s="2" t="n">
+      <c r="K11" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="L11" s="1" t="n">
         <v>99.5225273083084</v>
       </c>
-      <c r="M11" s="2" t="n">
+      <c r="M11" s="1" t="n">
         <v>0.749644859282492</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="N11" s="1" t="n">
         <v>22.4521446861513</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="O11" s="1" t="n">
         <v>0.749644859282492</v>
       </c>
-      <c r="P11" s="2" t="n">
+      <c r="P11" s="1" t="n">
         <v>59.715788716297</v>
       </c>
-      <c r="S11" s="2" t="n">
-        <v>0.700545785025913</v>
-      </c>
-      <c r="T11" s="2" t="n">
+      <c r="S11" s="1" t="n">
+        <v>0.700545785025913</v>
+      </c>
+      <c r="T11" s="1" t="n">
         <v>297.602809197731</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.900227517476009</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="1" t="n">
         <v>38.1179319685312</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="1" t="n">
         <v>0.801917215853616</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="1" t="n">
         <v>-40.3945415747118</v>
       </c>
-      <c r="M12" s="2" t="n">
+      <c r="M12" s="1" t="n">
         <v>0.801917215853616</v>
       </c>
-      <c r="N12" s="2" t="n">
+      <c r="N12" s="1" t="n">
         <v>33.4537356044126</v>
       </c>
-      <c r="O12" s="2" t="n">
+      <c r="O12" s="1" t="n">
         <v>0.801917215853616</v>
       </c>
-      <c r="P12" s="2" t="n">
+      <c r="P12" s="1" t="n">
         <v>44.8800691802662</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="1" t="n">
         <v>257.787494226066</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="1" t="n">
         <v>0.849436782010227</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="1" t="n">
         <v>-32.2812680547922</v>
       </c>
-      <c r="M13" s="2" t="n">
+      <c r="M13" s="1" t="n">
         <v>0.849436782010227</v>
       </c>
-      <c r="N13" s="2" t="n">
+      <c r="N13" s="1" t="n">
         <v>36.5528492192871</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="O13" s="1" t="n">
         <v>0.849436782010227</v>
       </c>
-      <c r="P13" s="2" t="n">
+      <c r="P13" s="1" t="n">
         <v>33.6291487405397</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="1" t="n">
         <v>0.900227517476009</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="1" t="n">
         <v>-8.05613662223124</v>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="M14" s="1" t="n">
         <v>0.900227517476009</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="N14" s="1" t="n">
         <v>23.9883717547452</v>
       </c>
-      <c r="O14" s="2" t="n">
+      <c r="O14" s="1" t="n">
         <v>0.900227517476009</v>
       </c>
-      <c r="P14" s="2" t="n">
+      <c r="P14" s="1" t="n">
         <v>14.9570741166487</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="1" t="n">
         <v>0.950390241271653</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="1" t="n">
         <v>46.0339033127771</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="1" t="n">
         <v>124.856597801184</v>
       </c>
     </row>

</xml_diff>